<commit_message>
Added feature for CRUD City Management
</commit_message>
<xml_diff>
--- a/dump/List Logic v2.xlsx
+++ b/dump/List Logic v2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\tomcat\webapps\travel-portal\dump\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DB37DE68-46F6-4D3D-A69C-E690FC307A29}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{75EEE1B8-790D-4ACE-9665-9930F3F2162E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="20610" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -579,72 +579,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -675,6 +609,72 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B61" activeCellId="1" sqref="B63:D63 B61:D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,12 +1029,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
@@ -1049,67 +1049,67 @@
       <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="44">
+      <c r="A3" s="52">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="49"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="45"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="51"/>
       <c r="C4" s="46"/>
       <c r="D4" s="47"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="44">
+      <c r="A5" s="52">
         <v>2</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="40"/>
+      <c r="D5" s="49"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="45"/>
-      <c r="B6" s="27"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="46"/>
       <c r="D6" s="47"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="44">
+      <c r="A7" s="52">
         <v>3</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="40"/>
+      <c r="D7" s="49"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="45"/>
-      <c r="B8" s="27"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="46"/>
       <c r="D8" s="47"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="43"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="57"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -1126,80 +1126,80 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="48">
+      <c r="A12" s="26">
         <v>1</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="29" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="52"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="54" t="s">
+      <c r="A13" s="30"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="55" t="s">
+      <c r="D13" s="33" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="56">
+      <c r="A14" s="34">
         <v>2</v>
       </c>
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="58" t="s">
+      <c r="C14" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="59" t="s">
+      <c r="D14" s="37" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="50" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="51" t="s">
+      <c r="D15" s="29" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="50" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="51" t="s">
+      <c r="D16" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="50" t="s">
+      <c r="A17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="D17" s="29" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="50" t="s">
+      <c r="A18" s="26"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="51" t="s">
+      <c r="D18" s="29" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1332,66 +1332,66 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="60">
+      <c r="A31" s="38">
         <v>5</v>
       </c>
-      <c r="B31" s="61" t="s">
+      <c r="B31" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="62" t="s">
+      <c r="C31" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="63" t="s">
+      <c r="D31" s="41" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="64"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="66" t="s">
+      <c r="A32" s="42"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="67" t="s">
+      <c r="D32" s="45" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="64"/>
-      <c r="B33" s="65"/>
-      <c r="C33" s="66" t="s">
+      <c r="A33" s="42"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="67" t="s">
+      <c r="D33" s="45" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="64"/>
-      <c r="B34" s="65"/>
-      <c r="C34" s="66" t="s">
+      <c r="A34" s="42"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="67" t="s">
+      <c r="D34" s="45" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="64"/>
-      <c r="B35" s="65"/>
-      <c r="C35" s="66" t="s">
+      <c r="A35" s="42"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="67" t="s">
+      <c r="D35" s="45" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="64"/>
-      <c r="B36" s="65"/>
-      <c r="C36" s="66" t="s">
+      <c r="A36" s="42"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="67" t="s">
+      <c r="D36" s="45" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1484,50 +1484,50 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="9">
+      <c r="A45" s="38">
         <v>8</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D45" s="41" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="11"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="8" t="s">
+      <c r="A46" s="42"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="D46" s="25" t="s">
+      <c r="D46" s="45" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="9">
+      <c r="A47" s="38">
         <v>9</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="D47" s="19" t="s">
+      <c r="D47" s="41" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="11"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="8" t="s">
+      <c r="A48" s="42"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="D48" s="25" t="s">
+      <c r="D48" s="45" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1605,87 +1605,87 @@
     </row>
     <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="18"/>
-      <c r="B55" s="34" t="s">
+      <c r="B55" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="C55" s="35"/>
-      <c r="D55" s="36"/>
+      <c r="C55" s="59"/>
+      <c r="D55" s="60"/>
     </row>
     <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="18"/>
-      <c r="B56" s="34" t="s">
+      <c r="B56" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="35"/>
-      <c r="D56" s="36"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="60"/>
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="18"/>
-      <c r="B57" s="34" t="s">
+      <c r="B57" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="C57" s="35"/>
-      <c r="D57" s="36"/>
+      <c r="C57" s="59"/>
+      <c r="D57" s="60"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="18"/>
-      <c r="B58" s="34" t="s">
+      <c r="B58" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C58" s="35"/>
-      <c r="D58" s="36"/>
+      <c r="C58" s="59"/>
+      <c r="D58" s="60"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="18"/>
-      <c r="B59" s="34" t="s">
+      <c r="B59" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="35"/>
-      <c r="D59" s="36"/>
+      <c r="C59" s="59"/>
+      <c r="D59" s="60"/>
     </row>
     <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="18"/>
-      <c r="B60" s="34" t="s">
+      <c r="B60" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="C60" s="35"/>
-      <c r="D60" s="36"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="60"/>
     </row>
     <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="18"/>
-      <c r="B61" s="34" t="s">
+      <c r="B61" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C61" s="35"/>
-      <c r="D61" s="36"/>
+      <c r="C61" s="59"/>
+      <c r="D61" s="60"/>
     </row>
     <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
-      <c r="B62" s="34" t="s">
+      <c r="B62" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="C62" s="35"/>
-      <c r="D62" s="36"/>
+      <c r="C62" s="59"/>
+      <c r="D62" s="60"/>
     </row>
     <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="18"/>
-      <c r="B63" s="34" t="s">
+      <c r="B63" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C63" s="35"/>
-      <c r="D63" s="36"/>
+      <c r="C63" s="59"/>
+      <c r="D63" s="60"/>
     </row>
     <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="18"/>
-      <c r="B64" s="34"/>
-      <c r="C64" s="35"/>
-      <c r="D64" s="36"/>
+      <c r="B64" s="58"/>
+      <c r="C64" s="59"/>
+      <c r="D64" s="60"/>
     </row>
     <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="18"/>
-      <c r="B65" s="34"/>
-      <c r="C65" s="35"/>
-      <c r="D65" s="36"/>
+      <c r="B65" s="58"/>
+      <c r="C65" s="59"/>
+      <c r="D65" s="60"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
@@ -1739,21 +1739,21 @@
       <c r="A72" s="13"/>
     </row>
     <row r="73" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="41" t="s">
+      <c r="A73" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B73" s="42"/>
-      <c r="C73" s="42"/>
-      <c r="D73" s="43"/>
+      <c r="B73" s="56"/>
+      <c r="C73" s="56"/>
+      <c r="D73" s="57"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="26">
+      <c r="A74" s="50">
         <v>1</v>
       </c>
-      <c r="B74" s="30" t="s">
+      <c r="B74" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="C74" s="26">
+      <c r="C74" s="50">
         <v>5</v>
       </c>
       <c r="D74" s="6" t="s">
@@ -1761,51 +1761,51 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="32"/>
-      <c r="B75" s="33"/>
-      <c r="C75" s="32"/>
+      <c r="A75" s="61"/>
+      <c r="B75" s="64"/>
+      <c r="C75" s="61"/>
       <c r="D75" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="32"/>
-      <c r="B76" s="33"/>
-      <c r="C76" s="32"/>
-      <c r="D76" s="8" t="s">
+      <c r="A76" s="61"/>
+      <c r="B76" s="64"/>
+      <c r="C76" s="61"/>
+      <c r="D76" s="28" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="32"/>
-      <c r="B77" s="33"/>
-      <c r="C77" s="32"/>
+      <c r="A77" s="61"/>
+      <c r="B77" s="64"/>
+      <c r="C77" s="61"/>
       <c r="D77" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="32"/>
-      <c r="B78" s="33"/>
-      <c r="C78" s="32"/>
-      <c r="D78" s="66" t="s">
+      <c r="A78" s="61"/>
+      <c r="B78" s="64"/>
+      <c r="C78" s="61"/>
+      <c r="D78" s="44" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="27"/>
-      <c r="B79" s="31"/>
-      <c r="C79" s="27"/>
+      <c r="A79" s="51"/>
+      <c r="B79" s="65"/>
+      <c r="C79" s="51"/>
       <c r="D79" s="7"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="26">
+      <c r="A80" s="50">
         <v>2</v>
       </c>
-      <c r="B80" s="30" t="s">
+      <c r="B80" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C80" s="37" t="s">
+      <c r="C80" s="62" t="s">
         <v>36</v>
       </c>
       <c r="D80" s="6" t="s">
@@ -1813,43 +1813,43 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="32"/>
-      <c r="B81" s="33"/>
-      <c r="C81" s="32"/>
+      <c r="A81" s="61"/>
+      <c r="B81" s="64"/>
+      <c r="C81" s="61"/>
       <c r="D81" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="32"/>
-      <c r="B82" s="33"/>
-      <c r="C82" s="32"/>
-      <c r="D82" s="8" t="s">
+      <c r="A82" s="61"/>
+      <c r="B82" s="64"/>
+      <c r="C82" s="61"/>
+      <c r="D82" s="44" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="32"/>
-      <c r="B83" s="33"/>
-      <c r="C83" s="32"/>
+      <c r="A83" s="61"/>
+      <c r="B83" s="64"/>
+      <c r="C83" s="61"/>
       <c r="D83" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="27"/>
-      <c r="B84" s="31"/>
-      <c r="C84" s="27"/>
+      <c r="A84" s="51"/>
+      <c r="B84" s="65"/>
+      <c r="C84" s="51"/>
       <c r="D84" s="7"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="26">
+      <c r="A85" s="50">
         <v>3</v>
       </c>
-      <c r="B85" s="30" t="s">
+      <c r="B85" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="C85" s="37" t="s">
+      <c r="C85" s="62" t="s">
         <v>36</v>
       </c>
       <c r="D85" s="6" t="s">
@@ -1857,43 +1857,43 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="32"/>
-      <c r="B86" s="33"/>
-      <c r="C86" s="32"/>
+      <c r="A86" s="61"/>
+      <c r="B86" s="64"/>
+      <c r="C86" s="61"/>
       <c r="D86" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="32"/>
-      <c r="B87" s="33"/>
-      <c r="C87" s="32"/>
-      <c r="D87" s="8" t="s">
+      <c r="A87" s="61"/>
+      <c r="B87" s="64"/>
+      <c r="C87" s="61"/>
+      <c r="D87" s="44" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="32"/>
-      <c r="B88" s="33"/>
-      <c r="C88" s="32"/>
+      <c r="A88" s="61"/>
+      <c r="B88" s="64"/>
+      <c r="C88" s="61"/>
       <c r="D88" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="27"/>
-      <c r="B89" s="31"/>
-      <c r="C89" s="27"/>
+      <c r="A89" s="51"/>
+      <c r="B89" s="65"/>
+      <c r="C89" s="51"/>
       <c r="D89" s="7"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="26">
+      <c r="A90" s="50">
         <v>4</v>
       </c>
-      <c r="B90" s="30" t="s">
+      <c r="B90" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C90" s="37" t="s">
+      <c r="C90" s="62" t="s">
         <v>35</v>
       </c>
       <c r="D90" s="6" t="s">
@@ -1901,46 +1901,46 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="32"/>
-      <c r="B91" s="33"/>
-      <c r="C91" s="32"/>
+      <c r="A91" s="61"/>
+      <c r="B91" s="64"/>
+      <c r="C91" s="61"/>
       <c r="D91" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="32"/>
-      <c r="B92" s="33"/>
-      <c r="C92" s="32"/>
-      <c r="D92" s="8" t="s">
+      <c r="A92" s="61"/>
+      <c r="B92" s="64"/>
+      <c r="C92" s="61"/>
+      <c r="D92" s="44" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="27"/>
-      <c r="B93" s="31"/>
-      <c r="C93" s="27"/>
+      <c r="A93" s="51"/>
+      <c r="B93" s="65"/>
+      <c r="C93" s="51"/>
       <c r="D93" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="95" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="41" t="s">
+      <c r="A95" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B95" s="42"/>
-      <c r="C95" s="42"/>
-      <c r="D95" s="43"/>
+      <c r="B95" s="56"/>
+      <c r="C95" s="56"/>
+      <c r="D95" s="57"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="26">
+      <c r="A96" s="50">
         <v>1</v>
       </c>
-      <c r="B96" s="30" t="s">
+      <c r="B96" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="C96" s="26">
+      <c r="C96" s="50">
         <v>1</v>
       </c>
       <c r="D96" s="6" t="s">
@@ -1948,25 +1948,25 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="32"/>
-      <c r="B97" s="33"/>
-      <c r="C97" s="32"/>
+      <c r="A97" s="61"/>
+      <c r="B97" s="64"/>
+      <c r="C97" s="61"/>
       <c r="D97" s="8"/>
     </row>
     <row r="98" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="27"/>
-      <c r="B98" s="31"/>
-      <c r="C98" s="27"/>
+      <c r="A98" s="51"/>
+      <c r="B98" s="65"/>
+      <c r="C98" s="51"/>
       <c r="D98" s="7"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="26">
+      <c r="A99" s="50">
         <v>2</v>
       </c>
-      <c r="B99" s="30" t="s">
+      <c r="B99" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="C99" s="28" t="s">
+      <c r="C99" s="66" t="s">
         <v>34</v>
       </c>
       <c r="D99" s="8" t="s">
@@ -1974,9 +1974,9 @@
       </c>
     </row>
     <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="27"/>
-      <c r="B100" s="31"/>
-      <c r="C100" s="29"/>
+      <c r="A100" s="51"/>
+      <c r="B100" s="65"/>
+      <c r="C100" s="67"/>
       <c r="D100" s="7" t="s">
         <v>45</v>
       </c>
@@ -1986,16 +1986,25 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="A90:A93"/>
+    <mergeCell ref="B90:B93"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="B96:B98"/>
+    <mergeCell ref="C96:C98"/>
+    <mergeCell ref="A74:A79"/>
+    <mergeCell ref="A80:A84"/>
+    <mergeCell ref="B80:B84"/>
+    <mergeCell ref="A85:A89"/>
+    <mergeCell ref="B85:B89"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="C74:C79"/>
+    <mergeCell ref="C80:C84"/>
+    <mergeCell ref="C85:C89"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="B74:B79"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A10:D10"/>
@@ -2012,25 +2021,16 @@
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="B64:D64"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="C74:C79"/>
-    <mergeCell ref="C80:C84"/>
-    <mergeCell ref="C85:C89"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="B74:B79"/>
-    <mergeCell ref="A74:A79"/>
-    <mergeCell ref="A80:A84"/>
-    <mergeCell ref="B80:B84"/>
-    <mergeCell ref="A85:A89"/>
-    <mergeCell ref="B85:B89"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="A90:A93"/>
-    <mergeCell ref="B90:B93"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="B96:B98"/>
-    <mergeCell ref="C96:C98"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Feature Ticket Transaction
</commit_message>
<xml_diff>
--- a/dump/List Logic v2.xlsx
+++ b/dump/List Logic v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\tomcat\webapps\travel-portal\dump\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EC356FF9-AE4F-47C0-82C2-9F52361BBFA0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2621EF1C-A940-46AB-A282-EA7A5BA98147}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="20610" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="85">
   <si>
     <t>No</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>required, numeric</t>
+  </si>
+  <si>
+    <t>Detail</t>
   </si>
 </sst>
 </file>
@@ -537,23 +540,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -565,7 +561,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -577,7 +572,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -608,72 +602,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -681,6 +609,80 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -689,6 +691,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1030,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F105" sqref="F105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,742 +1061,730 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="20"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="62">
+      <c r="A3" s="71">
         <v>1</v>
       </c>
       <c r="B3" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="58"/>
+      <c r="D3" s="64"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="63"/>
+      <c r="A4" s="72"/>
       <c r="B4" s="45"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="65"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="74"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="62">
+      <c r="A5" s="71">
         <v>2</v>
       </c>
       <c r="B5" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="58"/>
+      <c r="D5" s="64"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="63"/>
+      <c r="A6" s="72"/>
       <c r="B6" s="45"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="65"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="74"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="62">
+      <c r="A7" s="71">
         <v>3</v>
       </c>
       <c r="B7" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="58"/>
+      <c r="D7" s="64"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="63"/>
+      <c r="A8" s="72"/>
       <c r="B8" s="45"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="65"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="67"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="24">
+      <c r="A12" s="19">
         <v>1</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="22" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="30" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="26" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="32">
+      <c r="A14" s="27">
         <v>2</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="30" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26" t="s">
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="22" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26" t="s">
+      <c r="A16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="22" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="26" t="s">
+      <c r="A17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="22" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="26" t="s">
+      <c r="A18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="22" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="36">
+      <c r="A19" s="31">
         <v>3</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="33" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="42" t="s">
+      <c r="A20" s="35"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="37" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="42" t="s">
+      <c r="A21" s="35"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="37" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="42" t="s">
+      <c r="A22" s="35"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="37" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="42" t="s">
+      <c r="A23" s="35"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="37" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="40"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="42" t="s">
+      <c r="A24" s="35"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="37" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="40"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="42" t="s">
+      <c r="A25" s="35"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="42" t="s">
+      <c r="D25" s="37" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="36">
+      <c r="A26" s="31">
         <v>4</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="38" t="s">
+      <c r="D26" s="33" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="40"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="42" t="s">
+      <c r="A27" s="35"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="37" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="42" t="s">
+      <c r="A28" s="35"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="37" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="42" t="s">
+      <c r="A29" s="35"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="37" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="42" t="s">
+      <c r="A30" s="35"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="42" t="s">
+      <c r="D30" s="37" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="40"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="42" t="s">
+      <c r="A31" s="35"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="42" t="s">
+      <c r="D31" s="37" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="66"/>
-      <c r="B32" s="67"/>
-      <c r="C32" s="42" t="s">
+      <c r="A32" s="39"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="42" t="s">
+      <c r="D32" s="37" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="36">
+      <c r="A33" s="31">
         <v>5</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="38" t="s">
+      <c r="C33" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="39" t="s">
+      <c r="D33" s="34" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="40"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="42" t="s">
+      <c r="A34" s="35"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="43" t="s">
+      <c r="D34" s="38" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="40"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="42" t="s">
+      <c r="A35" s="35"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="43" t="s">
+      <c r="D35" s="38" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="40"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="42" t="s">
+      <c r="A36" s="35"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="43" t="s">
+      <c r="D36" s="38" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="40"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="42" t="s">
+      <c r="A37" s="35"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="43" t="s">
+      <c r="D37" s="38" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="40"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="42" t="s">
+      <c r="A38" s="35"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="D38" s="43" t="s">
+      <c r="D38" s="38" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="36">
+      <c r="A39" s="31">
         <v>6</v>
       </c>
-      <c r="B39" s="37" t="s">
+      <c r="B39" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C39" s="38" t="s">
+      <c r="C39" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D39" s="39" t="s">
+      <c r="D39" s="34" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="40"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="42" t="s">
+      <c r="A40" s="35"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="43" t="s">
+      <c r="D40" s="38" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="40"/>
-      <c r="B41" s="41"/>
-      <c r="C41" s="42" t="s">
+      <c r="A41" s="35"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="43" t="s">
+      <c r="D41" s="38" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="40"/>
-      <c r="B42" s="41"/>
-      <c r="C42" s="42" t="s">
+      <c r="A42" s="35"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="43" t="s">
+      <c r="D42" s="38" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="36">
+      <c r="A43" s="31">
         <v>7</v>
       </c>
-      <c r="B43" s="37" t="s">
+      <c r="B43" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="38" t="s">
+      <c r="C43" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D43" s="39" t="s">
+      <c r="D43" s="34" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="40"/>
-      <c r="B44" s="41"/>
-      <c r="C44" s="42" t="s">
+      <c r="A44" s="35"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="43" t="s">
+      <c r="D44" s="38" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="40"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="42" t="s">
+      <c r="A45" s="35"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D45" s="43" t="s">
+      <c r="D45" s="38" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="40"/>
-      <c r="B46" s="41"/>
-      <c r="C46" s="42" t="s">
+      <c r="A46" s="35"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="43" t="s">
+      <c r="D46" s="38" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="36">
+      <c r="A47" s="31">
         <v>8</v>
       </c>
-      <c r="B47" s="37" t="s">
+      <c r="B47" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="38" t="s">
+      <c r="C47" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="D47" s="39" t="s">
+      <c r="D47" s="34" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="40"/>
-      <c r="B48" s="41"/>
-      <c r="C48" s="42" t="s">
+      <c r="A48" s="35"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="D48" s="43" t="s">
+      <c r="D48" s="38" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="36">
+      <c r="A49" s="31">
         <v>9</v>
       </c>
-      <c r="B49" s="37" t="s">
+      <c r="B49" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="C49" s="38" t="s">
+      <c r="C49" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="D49" s="39" t="s">
+      <c r="D49" s="34" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="40"/>
-      <c r="B50" s="41"/>
-      <c r="C50" s="42" t="s">
+      <c r="A50" s="35"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="D50" s="43" t="s">
+      <c r="D50" s="38" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="8">
+      <c r="A51" s="31">
         <v>10</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="D51" s="17" t="s">
+      <c r="D51" s="34" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="9"/>
-      <c r="B52" s="4" t="s">
+      <c r="A52" s="35"/>
+      <c r="B52" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="D52" s="23" t="s">
+      <c r="D52" s="38" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="9"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="7" t="s">
+      <c r="A53" s="35"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="D53" s="23" t="s">
+      <c r="D53" s="38" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="8">
+      <c r="A54" s="31">
         <v>11</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D54" s="17" t="s">
-        <v>77</v>
-      </c>
+      <c r="C54" s="33"/>
+      <c r="D54" s="34"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="9"/>
-      <c r="B55" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D55" s="23" t="s">
-        <v>79</v>
-      </c>
+      <c r="A55" s="35"/>
+      <c r="B55" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C55" s="37"/>
+      <c r="D55" s="38"/>
     </row>
     <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="9"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D56" s="23" t="s">
-        <v>81</v>
-      </c>
+      <c r="A56" s="35"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="38"/>
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="68"/>
-      <c r="B57" s="69" t="s">
+      <c r="A57" s="41"/>
+      <c r="B57" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="70"/>
-      <c r="D57" s="71"/>
+      <c r="C57" s="69"/>
+      <c r="D57" s="70"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="68"/>
-      <c r="B58" s="69" t="s">
+      <c r="A58" s="41"/>
+      <c r="B58" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="70"/>
-      <c r="D58" s="71"/>
+      <c r="C58" s="69"/>
+      <c r="D58" s="70"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="68"/>
-      <c r="B59" s="69" t="s">
+      <c r="A59" s="41"/>
+      <c r="B59" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="C59" s="70"/>
-      <c r="D59" s="71"/>
+      <c r="C59" s="69"/>
+      <c r="D59" s="70"/>
     </row>
     <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="68"/>
-      <c r="B60" s="69" t="s">
+      <c r="A60" s="41"/>
+      <c r="B60" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="C60" s="70"/>
-      <c r="D60" s="71"/>
+      <c r="C60" s="69"/>
+      <c r="D60" s="70"/>
     </row>
     <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="16"/>
-      <c r="B61" s="52" t="s">
+      <c r="A61" s="13"/>
+      <c r="B61" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="C61" s="53"/>
-      <c r="D61" s="54"/>
+      <c r="C61" s="59"/>
+      <c r="D61" s="60"/>
     </row>
     <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="68"/>
-      <c r="B62" s="69" t="s">
+      <c r="A62" s="41"/>
+      <c r="B62" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C62" s="70"/>
-      <c r="D62" s="71"/>
+      <c r="C62" s="69"/>
+      <c r="D62" s="70"/>
     </row>
     <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="16"/>
-      <c r="B63" s="52" t="s">
+      <c r="A63" s="13"/>
+      <c r="B63" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C63" s="53"/>
-      <c r="D63" s="54"/>
+      <c r="C63" s="59"/>
+      <c r="D63" s="60"/>
     </row>
     <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="68"/>
-      <c r="B64" s="69" t="s">
+      <c r="A64" s="41"/>
+      <c r="B64" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="C64" s="70"/>
-      <c r="D64" s="71"/>
+      <c r="C64" s="69"/>
+      <c r="D64" s="70"/>
     </row>
     <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="16"/>
-      <c r="B65" s="52" t="s">
+      <c r="A65" s="13"/>
+      <c r="B65" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C65" s="53"/>
-      <c r="D65" s="54"/>
+      <c r="C65" s="59"/>
+      <c r="D65" s="60"/>
     </row>
     <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="16"/>
-      <c r="B66" s="52"/>
-      <c r="C66" s="53"/>
-      <c r="D66" s="54"/>
+      <c r="A66" s="13"/>
+      <c r="B66" s="58"/>
+      <c r="C66" s="59"/>
+      <c r="D66" s="60"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="16"/>
-      <c r="B67" s="52"/>
-      <c r="C67" s="53"/>
-      <c r="D67" s="54"/>
+      <c r="A67" s="13"/>
+      <c r="B67" s="58"/>
+      <c r="C67" s="59"/>
+      <c r="D67" s="60"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="11"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
+      <c r="A68" s="8"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="11"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
+      <c r="A69" s="8"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="11"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="12"/>
+      <c r="A70" s="8"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="11"/>
-      <c r="B71" s="14" t="s">
+      <c r="A71" s="8"/>
+      <c r="B71" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C71" s="15"/>
-      <c r="D71" s="15"/>
-      <c r="E71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="9"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="11"/>
-      <c r="B72" s="14" t="s">
+      <c r="A72" s="8"/>
+      <c r="B72" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="15"/>
-      <c r="E72" s="12"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="9"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="11"/>
-      <c r="B73" s="14" t="s">
+      <c r="A73" s="8"/>
+      <c r="B73" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C73" s="15"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="12"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="9"/>
     </row>
     <row r="74" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="11"/>
+      <c r="A74" s="8"/>
     </row>
     <row r="75" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="59" t="s">
+      <c r="A75" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B75" s="60"/>
-      <c r="C75" s="60"/>
-      <c r="D75" s="61"/>
+      <c r="B75" s="66"/>
+      <c r="C75" s="66"/>
+      <c r="D75" s="67"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="44">
@@ -1791,7 +1796,7 @@
       <c r="C76" s="44">
         <v>5</v>
       </c>
-      <c r="D76" s="38" t="s">
+      <c r="D76" s="33" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1799,7 +1804,7 @@
       <c r="A77" s="50"/>
       <c r="B77" s="51"/>
       <c r="C77" s="50"/>
-      <c r="D77" s="42" t="s">
+      <c r="D77" s="37" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1807,7 +1812,7 @@
       <c r="A78" s="50"/>
       <c r="B78" s="51"/>
       <c r="C78" s="50"/>
-      <c r="D78" s="26" t="s">
+      <c r="D78" s="21" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1815,7 +1820,7 @@
       <c r="A79" s="50"/>
       <c r="B79" s="51"/>
       <c r="C79" s="50"/>
-      <c r="D79" s="7" t="s">
+      <c r="D79" s="37" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1823,7 +1828,7 @@
       <c r="A80" s="50"/>
       <c r="B80" s="51"/>
       <c r="C80" s="50"/>
-      <c r="D80" s="42" t="s">
+      <c r="D80" s="37" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1831,7 +1836,7 @@
       <c r="A81" s="45"/>
       <c r="B81" s="49"/>
       <c r="C81" s="45"/>
-      <c r="D81" s="6"/>
+      <c r="D81" s="42"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="44">
@@ -1840,10 +1845,10 @@
       <c r="B82" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C82" s="55" t="s">
+      <c r="C82" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="D82" s="38" t="s">
+      <c r="D82" s="33" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1851,7 +1856,7 @@
       <c r="A83" s="50"/>
       <c r="B83" s="51"/>
       <c r="C83" s="50"/>
-      <c r="D83" s="42" t="s">
+      <c r="D83" s="37" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1859,7 +1864,7 @@
       <c r="A84" s="50"/>
       <c r="B84" s="51"/>
       <c r="C84" s="50"/>
-      <c r="D84" s="42" t="s">
+      <c r="D84" s="37" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1867,7 +1872,7 @@
       <c r="A85" s="50"/>
       <c r="B85" s="51"/>
       <c r="C85" s="50"/>
-      <c r="D85" s="7" t="s">
+      <c r="D85" s="37" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1875,7 +1880,7 @@
       <c r="A86" s="45"/>
       <c r="B86" s="49"/>
       <c r="C86" s="45"/>
-      <c r="D86" s="6"/>
+      <c r="D86" s="42"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="44">
@@ -1884,10 +1889,10 @@
       <c r="B87" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C87" s="55" t="s">
+      <c r="C87" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="D87" s="38" t="s">
+      <c r="D87" s="33" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1895,7 +1900,7 @@
       <c r="A88" s="50"/>
       <c r="B88" s="51"/>
       <c r="C88" s="50"/>
-      <c r="D88" s="42" t="s">
+      <c r="D88" s="37" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1903,7 +1908,7 @@
       <c r="A89" s="50"/>
       <c r="B89" s="51"/>
       <c r="C89" s="50"/>
-      <c r="D89" s="42" t="s">
+      <c r="D89" s="37" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1911,7 +1916,7 @@
       <c r="A90" s="50"/>
       <c r="B90" s="51"/>
       <c r="C90" s="50"/>
-      <c r="D90" s="7" t="s">
+      <c r="D90" s="37" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1919,7 +1924,7 @@
       <c r="A91" s="45"/>
       <c r="B91" s="49"/>
       <c r="C91" s="45"/>
-      <c r="D91" s="6"/>
+      <c r="D91" s="42"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="44">
@@ -1928,10 +1933,10 @@
       <c r="B92" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C92" s="55" t="s">
+      <c r="C92" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="D92" s="38" t="s">
+      <c r="D92" s="33" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1939,7 +1944,7 @@
       <c r="A93" s="50"/>
       <c r="B93" s="51"/>
       <c r="C93" s="50"/>
-      <c r="D93" s="42" t="s">
+      <c r="D93" s="37" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1947,7 +1952,7 @@
       <c r="A94" s="50"/>
       <c r="B94" s="51"/>
       <c r="C94" s="50"/>
-      <c r="D94" s="42" t="s">
+      <c r="D94" s="37" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1955,44 +1960,46 @@
       <c r="A95" s="45"/>
       <c r="B95" s="49"/>
       <c r="C95" s="45"/>
-      <c r="D95" s="6" t="s">
+      <c r="D95" s="43" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="97" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="59" t="s">
+      <c r="A97" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="B97" s="60"/>
-      <c r="C97" s="60"/>
-      <c r="D97" s="61"/>
+      <c r="B97" s="66"/>
+      <c r="C97" s="66"/>
+      <c r="D97" s="67"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="44">
+      <c r="A98" s="52">
         <v>1</v>
       </c>
-      <c r="B98" s="48" t="s">
+      <c r="B98" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C98" s="44">
+      <c r="C98" s="52">
         <v>1</v>
       </c>
-      <c r="D98" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="50"/>
-      <c r="B99" s="51"/>
-      <c r="C99" s="50"/>
-      <c r="D99" s="7"/>
+      <c r="D98" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="53"/>
+      <c r="B99" s="56"/>
+      <c r="C99" s="53"/>
+      <c r="D99" s="6"/>
     </row>
     <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="45"/>
-      <c r="B100" s="49"/>
-      <c r="C100" s="45"/>
-      <c r="D100" s="6"/>
+      <c r="A100" s="54"/>
+      <c r="B100" s="57"/>
+      <c r="C100" s="54"/>
+      <c r="D100" s="75">
+        <v>1</v>
+      </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="44">
@@ -2004,7 +2011,7 @@
       <c r="C101" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="D101" s="7" t="s">
+      <c r="D101" s="37" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2012,12 +2019,12 @@
       <c r="A102" s="45"/>
       <c r="B102" s="49"/>
       <c r="C102" s="47"/>
-      <c r="D102" s="6" t="s">
+      <c r="D102" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="13"/>
+      <c r="B103" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="45">

</xml_diff>

<commit_message>
feature(TrackOrder): Added feature for tracking order by entered Invoice Number
</commit_message>
<xml_diff>
--- a/dump/List Logic v2.xlsx
+++ b/dump/List Logic v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\tomcat\webapps\travel-portal\dump\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2621EF1C-A940-46AB-A282-EA7A5BA98147}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5D007B1E-15B1-4E8B-A045-EF88D3EC4A5F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="20610" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -540,16 +540,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -611,100 +608,83 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="0" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1047,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F105" sqref="F105"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,983 +1041,992 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="16"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="71">
+      <c r="A3" s="47">
         <v>1</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="64"/>
+      <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="74"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="71">
+      <c r="A5" s="47">
         <v>2</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="64"/>
+      <c r="D5" s="44"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="72"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="74"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="71">
+      <c r="A7" s="47">
         <v>3</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="64"/>
+      <c r="D7" s="44"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="72"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="74"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="67"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="52"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="A12" s="16">
         <v>1</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="19" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="23" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="27">
+      <c r="A14" s="24">
         <v>2</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="27" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="19" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="21" t="s">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21" t="s">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="19" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21" t="s">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="31">
+      <c r="A19" s="28">
         <v>3</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="30" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="37" t="s">
+      <c r="A20" s="32"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="34" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="37" t="s">
+      <c r="A21" s="32"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="37" t="s">
+      <c r="D21" s="34" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="37" t="s">
+      <c r="A22" s="32"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="37" t="s">
+      <c r="D22" s="34" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="37" t="s">
+      <c r="A23" s="32"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="34" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="37" t="s">
+      <c r="A24" s="32"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="34" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="37" t="s">
+      <c r="A25" s="32"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="34" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="31">
+      <c r="A26" s="28">
         <v>4</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C26" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="30" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="37" t="s">
+      <c r="A27" s="32"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="37" t="s">
+      <c r="D27" s="34" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="37" t="s">
+      <c r="A28" s="32"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="37" t="s">
+      <c r="D28" s="34" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="37" t="s">
+      <c r="A29" s="32"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="37" t="s">
+      <c r="D29" s="34" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="37" t="s">
+      <c r="A30" s="32"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="37" t="s">
+      <c r="D30" s="34" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="37" t="s">
+      <c r="A31" s="32"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="37" t="s">
+      <c r="D31" s="34" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="39"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="37" t="s">
+      <c r="A32" s="36"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="34" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="31">
+      <c r="A33" s="28">
         <v>5</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="33" t="s">
+      <c r="C33" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="31" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="37" t="s">
+      <c r="A34" s="32"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="38" t="s">
+      <c r="D34" s="35" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="37" t="s">
+      <c r="A35" s="32"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="38" t="s">
+      <c r="D35" s="35" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="37" t="s">
+      <c r="A36" s="32"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="38" t="s">
+      <c r="D36" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="37" t="s">
+      <c r="A37" s="32"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="38" t="s">
+      <c r="D37" s="35" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="35"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="37" t="s">
+      <c r="A38" s="32"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="31">
+      <c r="A39" s="28">
         <v>6</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C39" s="33" t="s">
+      <c r="C39" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="D39" s="31" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="37" t="s">
+      <c r="A40" s="32"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="38" t="s">
+      <c r="D40" s="35" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="35"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="37" t="s">
+      <c r="A41" s="32"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="38" t="s">
+      <c r="D41" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="35"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="37" t="s">
+      <c r="A42" s="32"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="38" t="s">
+      <c r="D42" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="31">
+      <c r="A43" s="28">
         <v>7</v>
       </c>
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="33" t="s">
+      <c r="C43" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="D43" s="34" t="s">
+      <c r="D43" s="31" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="35"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="37" t="s">
+      <c r="A44" s="32"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="38" t="s">
+      <c r="D44" s="35" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="37" t="s">
+      <c r="A45" s="32"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="D45" s="38" t="s">
+      <c r="D45" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="35"/>
-      <c r="B46" s="36"/>
-      <c r="C46" s="37" t="s">
+      <c r="A46" s="32"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="38" t="s">
+      <c r="D46" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="31">
+      <c r="A47" s="28">
         <v>8</v>
       </c>
-      <c r="B47" s="32" t="s">
+      <c r="B47" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="33" t="s">
+      <c r="C47" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="D47" s="34" t="s">
+      <c r="D47" s="31" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="35"/>
-      <c r="B48" s="36"/>
-      <c r="C48" s="37" t="s">
+      <c r="A48" s="32"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="D48" s="38" t="s">
+      <c r="D48" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="31">
+      <c r="A49" s="28">
         <v>9</v>
       </c>
-      <c r="B49" s="32" t="s">
+      <c r="B49" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C49" s="33" t="s">
+      <c r="C49" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="D49" s="34" t="s">
+      <c r="D49" s="31" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="35"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="37" t="s">
+      <c r="A50" s="32"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="D50" s="38" t="s">
+      <c r="D50" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="31">
+      <c r="A51" s="28">
         <v>10</v>
       </c>
-      <c r="B51" s="32" t="s">
+      <c r="B51" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="C51" s="33" t="s">
+      <c r="C51" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="D51" s="34" t="s">
+      <c r="D51" s="31" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="35"/>
-      <c r="B52" s="36" t="s">
+      <c r="A52" s="32"/>
+      <c r="B52" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="C52" s="37" t="s">
+      <c r="C52" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="D52" s="38" t="s">
+      <c r="D52" s="35" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="35"/>
-      <c r="B53" s="36"/>
-      <c r="C53" s="37" t="s">
+      <c r="A53" s="32"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D53" s="38" t="s">
+      <c r="D53" s="35" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="31">
+      <c r="A54" s="28">
         <v>11</v>
       </c>
-      <c r="B54" s="32" t="s">
+      <c r="B54" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="C54" s="33"/>
-      <c r="D54" s="34"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="31"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="35"/>
-      <c r="B55" s="36" t="s">
+      <c r="A55" s="32"/>
+      <c r="B55" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="C55" s="37"/>
-      <c r="D55" s="38"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="35"/>
     </row>
     <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="35"/>
-      <c r="B56" s="36"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="38"/>
+      <c r="A56" s="32"/>
+      <c r="B56" s="33"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="35"/>
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="41"/>
-      <c r="B57" s="68" t="s">
+      <c r="A57" s="38"/>
+      <c r="B57" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="69"/>
-      <c r="D57" s="70"/>
+      <c r="C57" s="54"/>
+      <c r="D57" s="55"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="41"/>
-      <c r="B58" s="68" t="s">
+      <c r="A58" s="38"/>
+      <c r="B58" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="69"/>
-      <c r="D58" s="70"/>
+      <c r="C58" s="54"/>
+      <c r="D58" s="55"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="41"/>
-      <c r="B59" s="68" t="s">
+      <c r="A59" s="38"/>
+      <c r="B59" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="C59" s="69"/>
-      <c r="D59" s="70"/>
+      <c r="C59" s="54"/>
+      <c r="D59" s="55"/>
     </row>
     <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="41"/>
-      <c r="B60" s="68" t="s">
+      <c r="A60" s="38"/>
+      <c r="B60" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="C60" s="69"/>
-      <c r="D60" s="70"/>
+      <c r="C60" s="54"/>
+      <c r="D60" s="55"/>
     </row>
     <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="13"/>
-      <c r="B61" s="58" t="s">
+      <c r="A61" s="10"/>
+      <c r="B61" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="C61" s="59"/>
-      <c r="D61" s="60"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="58"/>
     </row>
     <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="41"/>
-      <c r="B62" s="68" t="s">
+      <c r="A62" s="38"/>
+      <c r="B62" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C62" s="69"/>
-      <c r="D62" s="70"/>
+      <c r="C62" s="54"/>
+      <c r="D62" s="55"/>
     </row>
     <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="13"/>
-      <c r="B63" s="58" t="s">
+      <c r="A63" s="10"/>
+      <c r="B63" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="C63" s="59"/>
-      <c r="D63" s="60"/>
+      <c r="C63" s="57"/>
+      <c r="D63" s="58"/>
     </row>
     <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="41"/>
-      <c r="B64" s="68" t="s">
+      <c r="A64" s="38"/>
+      <c r="B64" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C64" s="69"/>
-      <c r="D64" s="70"/>
+      <c r="C64" s="54"/>
+      <c r="D64" s="55"/>
     </row>
     <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="13"/>
-      <c r="B65" s="58" t="s">
+      <c r="A65" s="10"/>
+      <c r="B65" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="C65" s="59"/>
-      <c r="D65" s="60"/>
+      <c r="C65" s="57"/>
+      <c r="D65" s="58"/>
     </row>
     <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="13"/>
-      <c r="B66" s="58"/>
-      <c r="C66" s="59"/>
-      <c r="D66" s="60"/>
+      <c r="A66" s="10"/>
+      <c r="B66" s="56"/>
+      <c r="C66" s="57"/>
+      <c r="D66" s="58"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="13"/>
-      <c r="B67" s="58"/>
-      <c r="C67" s="59"/>
-      <c r="D67" s="60"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="56"/>
+      <c r="C67" s="57"/>
+      <c r="D67" s="58"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="8"/>
+      <c r="A68" s="5"/>
       <c r="B68" s="3"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="8"/>
+      <c r="A69" s="5"/>
       <c r="B69" s="3"/>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="8"/>
+      <c r="A70" s="5"/>
       <c r="B70" s="3"/>
-      <c r="C70" s="9"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="8"/>
-      <c r="B71" s="11" t="s">
+      <c r="A71" s="5"/>
+      <c r="B71" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="9"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="6"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="8"/>
-      <c r="B72" s="11" t="s">
+      <c r="A72" s="5"/>
+      <c r="B72" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="9"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="6"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="8"/>
-      <c r="B73" s="11" t="s">
+      <c r="A73" s="5"/>
+      <c r="B73" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
-      <c r="E73" s="9"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="6"/>
     </row>
     <row r="74" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="8"/>
+      <c r="A74" s="5"/>
     </row>
     <row r="75" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="65" t="s">
+      <c r="A75" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B75" s="66"/>
-      <c r="C75" s="66"/>
-      <c r="D75" s="67"/>
+      <c r="B75" s="51"/>
+      <c r="C75" s="51"/>
+      <c r="D75" s="52"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="44">
+      <c r="A76" s="45">
         <v>1</v>
       </c>
-      <c r="B76" s="48" t="s">
+      <c r="B76" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C76" s="44">
+      <c r="C76" s="45">
         <v>5</v>
       </c>
-      <c r="D76" s="33" t="s">
+      <c r="D76" s="30" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="50"/>
-      <c r="B77" s="51"/>
-      <c r="C77" s="50"/>
-      <c r="D77" s="37" t="s">
+      <c r="A77" s="59"/>
+      <c r="B77" s="62"/>
+      <c r="C77" s="59"/>
+      <c r="D77" s="34" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="50"/>
-      <c r="B78" s="51"/>
-      <c r="C78" s="50"/>
-      <c r="D78" s="21" t="s">
+      <c r="A78" s="59"/>
+      <c r="B78" s="62"/>
+      <c r="C78" s="59"/>
+      <c r="D78" s="18" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="50"/>
-      <c r="B79" s="51"/>
-      <c r="C79" s="50"/>
-      <c r="D79" s="37" t="s">
+      <c r="A79" s="59"/>
+      <c r="B79" s="62"/>
+      <c r="C79" s="59"/>
+      <c r="D79" s="34" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="50"/>
-      <c r="B80" s="51"/>
-      <c r="C80" s="50"/>
-      <c r="D80" s="37" t="s">
+      <c r="A80" s="59"/>
+      <c r="B80" s="62"/>
+      <c r="C80" s="59"/>
+      <c r="D80" s="34" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="45"/>
-      <c r="B81" s="49"/>
-      <c r="C81" s="45"/>
-      <c r="D81" s="42"/>
+      <c r="A81" s="46"/>
+      <c r="B81" s="63"/>
+      <c r="C81" s="46"/>
+      <c r="D81" s="39"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="44">
+      <c r="A82" s="45">
         <v>2</v>
       </c>
-      <c r="B82" s="48" t="s">
+      <c r="B82" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C82" s="61" t="s">
+      <c r="C82" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="D82" s="33" t="s">
+      <c r="D82" s="30" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="50"/>
-      <c r="B83" s="51"/>
-      <c r="C83" s="50"/>
-      <c r="D83" s="37" t="s">
+      <c r="A83" s="59"/>
+      <c r="B83" s="62"/>
+      <c r="C83" s="59"/>
+      <c r="D83" s="34" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="50"/>
-      <c r="B84" s="51"/>
-      <c r="C84" s="50"/>
-      <c r="D84" s="37" t="s">
+      <c r="A84" s="59"/>
+      <c r="B84" s="62"/>
+      <c r="C84" s="59"/>
+      <c r="D84" s="34" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="50"/>
-      <c r="B85" s="51"/>
-      <c r="C85" s="50"/>
-      <c r="D85" s="37" t="s">
+      <c r="A85" s="59"/>
+      <c r="B85" s="62"/>
+      <c r="C85" s="59"/>
+      <c r="D85" s="34" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="45"/>
-      <c r="B86" s="49"/>
-      <c r="C86" s="45"/>
-      <c r="D86" s="42"/>
+      <c r="A86" s="46"/>
+      <c r="B86" s="63"/>
+      <c r="C86" s="46"/>
+      <c r="D86" s="39"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="44">
+      <c r="A87" s="45">
         <v>3</v>
       </c>
-      <c r="B87" s="48" t="s">
+      <c r="B87" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C87" s="61" t="s">
+      <c r="C87" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="D87" s="33" t="s">
+      <c r="D87" s="30" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="50"/>
-      <c r="B88" s="51"/>
-      <c r="C88" s="50"/>
-      <c r="D88" s="37" t="s">
+      <c r="A88" s="59"/>
+      <c r="B88" s="62"/>
+      <c r="C88" s="59"/>
+      <c r="D88" s="34" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="50"/>
-      <c r="B89" s="51"/>
-      <c r="C89" s="50"/>
-      <c r="D89" s="37" t="s">
+      <c r="A89" s="59"/>
+      <c r="B89" s="62"/>
+      <c r="C89" s="59"/>
+      <c r="D89" s="34" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="50"/>
-      <c r="B90" s="51"/>
-      <c r="C90" s="50"/>
-      <c r="D90" s="37" t="s">
+      <c r="A90" s="59"/>
+      <c r="B90" s="62"/>
+      <c r="C90" s="59"/>
+      <c r="D90" s="34" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="45"/>
-      <c r="B91" s="49"/>
-      <c r="C91" s="45"/>
-      <c r="D91" s="42"/>
+      <c r="A91" s="46"/>
+      <c r="B91" s="63"/>
+      <c r="C91" s="46"/>
+      <c r="D91" s="39"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="44">
+      <c r="A92" s="45">
         <v>4</v>
       </c>
-      <c r="B92" s="48" t="s">
+      <c r="B92" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C92" s="61" t="s">
+      <c r="C92" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="D92" s="33" t="s">
+      <c r="D92" s="30" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="50"/>
-      <c r="B93" s="51"/>
-      <c r="C93" s="50"/>
-      <c r="D93" s="37" t="s">
+      <c r="A93" s="59"/>
+      <c r="B93" s="62"/>
+      <c r="C93" s="59"/>
+      <c r="D93" s="34" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="50"/>
-      <c r="B94" s="51"/>
-      <c r="C94" s="50"/>
-      <c r="D94" s="37" t="s">
+      <c r="A94" s="59"/>
+      <c r="B94" s="62"/>
+      <c r="C94" s="59"/>
+      <c r="D94" s="34" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="45"/>
-      <c r="B95" s="49"/>
-      <c r="C95" s="45"/>
-      <c r="D95" s="43" t="s">
+      <c r="A95" s="46"/>
+      <c r="B95" s="63"/>
+      <c r="C95" s="46"/>
+      <c r="D95" s="40" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="97" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="65" t="s">
+      <c r="A97" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="B97" s="66"/>
-      <c r="C97" s="66"/>
-      <c r="D97" s="67"/>
+      <c r="B97" s="51"/>
+      <c r="C97" s="51"/>
+      <c r="D97" s="52"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="52">
+      <c r="A98" s="45">
         <v>1</v>
       </c>
-      <c r="B98" s="55" t="s">
+      <c r="B98" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C98" s="52">
+      <c r="C98" s="45">
         <v>1</v>
       </c>
-      <c r="D98" s="4" t="s">
+      <c r="D98" s="30" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="53"/>
-      <c r="B99" s="56"/>
-      <c r="C99" s="53"/>
-      <c r="D99" s="6"/>
+      <c r="A99" s="59"/>
+      <c r="B99" s="62"/>
+      <c r="C99" s="59"/>
+      <c r="D99" s="66"/>
     </row>
     <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="54"/>
-      <c r="B100" s="57"/>
-      <c r="C100" s="54"/>
-      <c r="D100" s="75">
+      <c r="A100" s="46"/>
+      <c r="B100" s="63"/>
+      <c r="C100" s="46"/>
+      <c r="D100" s="67">
         <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="44">
+      <c r="A101" s="45">
         <v>2</v>
       </c>
-      <c r="B101" s="48" t="s">
+      <c r="B101" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="C101" s="46" t="s">
+      <c r="C101" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="D101" s="37" t="s">
+      <c r="D101" s="34" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="45"/>
-      <c r="B102" s="49"/>
-      <c r="C102" s="47"/>
-      <c r="D102" s="5" t="s">
+      <c r="A102" s="46"/>
+      <c r="B102" s="63"/>
+      <c r="C102" s="65"/>
+      <c r="D102" s="40" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="10"/>
+      <c r="B103" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A101:A102"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="B92:B95"/>
+    <mergeCell ref="A98:A100"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="C98:C100"/>
+    <mergeCell ref="A76:A81"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="A87:A91"/>
+    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="C76:C81"/>
+    <mergeCell ref="C82:C86"/>
+    <mergeCell ref="C87:C91"/>
+    <mergeCell ref="C92:C95"/>
+    <mergeCell ref="B76:B81"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A10:D10"/>
@@ -2054,25 +2043,16 @@
     <mergeCell ref="B64:D64"/>
     <mergeCell ref="B66:D66"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="C76:C81"/>
-    <mergeCell ref="C82:C86"/>
-    <mergeCell ref="C87:C91"/>
-    <mergeCell ref="C92:C95"/>
-    <mergeCell ref="B76:B81"/>
-    <mergeCell ref="A76:A81"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="A87:A91"/>
-    <mergeCell ref="B87:B91"/>
-    <mergeCell ref="A101:A102"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="B92:B95"/>
-    <mergeCell ref="A98:A100"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="C98:C100"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>